<commit_message>
Use cv::forEach to test.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
   <si>
     <t xml:space="preserve">inner OpenCV</t>
   </si>
@@ -34,6 +34,9 @@
   <si>
     <t xml:space="preserve">outer OpenMP</t>
   </si>
+  <si>
+    <t xml:space="preserve">forEach</t>
+  </si>
 </sst>
 </file>
 
@@ -42,11 +45,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -62,6 +66,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,9 +117,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -119,8 +134,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -140,10 +159,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -165,28 +184,28 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -194,22 +213,22 @@
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="I3" s="3"/>
+      <c r="B3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -327,13 +346,196 @@
         <v>31.65</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>46.07</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>27.14</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>17.45</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>23.56</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>23.55</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>12.33</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>12.34</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>12.27</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>12.29</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>7.13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>9.02</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>7.17</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>9.03</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>7.18</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>9.18</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>7.19</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>9.2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -458,7 +660,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>